<commit_message>
init map super class methods
</commit_message>
<xml_diff>
--- a/cars.xlsx
+++ b/cars.xlsx
@@ -17,7 +17,7 @@
     <t>model</t>
   </si>
   <si>
-    <t>id</t>
+    <t>musta id</t>
   </si>
   <si>
     <t>foo</t>
@@ -38,13 +38,13 @@
     <t>My new model</t>
   </si>
   <si>
-    <t>22</t>
+    <t>24</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>2022-10-02</t>
+    <t>2022-10-03</t>
   </si>
   <si>
     <t/>

</xml_diff>

<commit_message>
add support for inherited static methods
</commit_message>
<xml_diff>
--- a/cars.xlsx
+++ b/cars.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>fofo</t>
   </si>
@@ -20,6 +20,18 @@
     <t>tototot</t>
   </si>
   <si>
+    <t>something</t>
+  </si>
+  <si>
+    <t>setNameFromAbstract</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>enumeration</t>
+  </si>
+  <si>
     <t>model</t>
   </si>
   <si>
@@ -38,9 +50,6 @@
     <t>price</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>nameFromAbstract</t>
   </si>
   <si>
@@ -50,22 +59,22 @@
     <t/>
   </si>
   <si>
+    <t>Porsche</t>
+  </si>
+  <si>
     <t>My new model</t>
   </si>
   <si>
     <t>24</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>2022-10-07</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2022-10-09</t>
   </si>
   <si>
     <t>300 000,99 MAD</t>
-  </si>
-  <si>
-    <t>Porsche</t>
   </si>
 </sst>
 </file>
@@ -110,7 +119,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -150,75 +159,102 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="K2" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="K3" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upgrade to java 17
</commit_message>
<xml_diff>
--- a/cars.xlsx
+++ b/cars.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
   <si>
     <t>price</t>
   </si>
@@ -29,6 +29,9 @@
     <t>fromAbstract</t>
   </si>
   <si>
+    <t>hhh</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
@@ -53,7 +56,7 @@
     <t>updateDate</t>
   </si>
   <si>
-    <t>300 000,99 MAD</t>
+    <t>300.000,99 MAD</t>
   </si>
   <si>
     <t/>
@@ -71,7 +74,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>Sun Oct 16 13:03:08 WEST 2022</t>
+    <t>Tue Sep 26 01:28:00 EDT 2023</t>
   </si>
 </sst>
 </file>
@@ -116,7 +119,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -165,40 +168,43 @@
       <c r="N1" t="s">
         <v>12</v>
       </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L2" t="s">
         <v>18</v>
@@ -207,42 +213,45 @@
         <v>19</v>
       </c>
       <c r="N2" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L3" t="s">
         <v>18</v>
@@ -251,7 +260,10 @@
         <v>19</v>
       </c>
       <c r="N3" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>